<commit_message>
Se libera version 1.04 de PLC y 1.04 de HMI
</commit_message>
<xml_diff>
--- a/Pruebas/texto.xlsx
+++ b/Pruebas/texto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="HEX" sheetId="5" r:id="rId1"/>
     <sheet name="TEXTO" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -41,16 +41,16 @@
     <t>41</t>
   </si>
   <si>
-    <t>Error=</t>
+    <t>HEXWORD</t>
   </si>
   <si>
-    <t>HEXWORD</t>
+    <t xml:space="preserve"> RH=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,17 +140,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,6 +161,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -209,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +247,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +633,7 @@
   <dimension ref="A3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -642,17 +645,17 @@
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="str">
         <f>B3 &amp; REPT(" ",10-LEN(B3))</f>
-        <v xml:space="preserve">Error=    </v>
+        <v xml:space="preserve"> RH=      </v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="4">
         <v>1</v>
       </c>
@@ -685,46 +688,46 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="11" t="str">
+      <c r="B8" s="9" t="str">
         <f>CHAR(B9)</f>
-        <v>E</v>
-      </c>
-      <c r="C8" s="11" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C8" s="9" t="str">
         <f t="shared" ref="C8:K8" si="0">CHAR(C9)</f>
-        <v>r</v>
-      </c>
-      <c r="D8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>r</v>
-      </c>
-      <c r="E8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
-      </c>
-      <c r="F8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>r</v>
-      </c>
-      <c r="G8" s="11" t="str">
+        <v>R</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>H</v>
+      </c>
+      <c r="E8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>=</v>
       </c>
-      <c r="H8" s="11" t="str">
+      <c r="F8" s="9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="G8" s="9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J8" s="11" t="str">
+      <c r="H8" s="9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K8" s="11" t="str">
+      <c r="I8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K8" s="9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
@@ -735,27 +738,27 @@
       </c>
       <c r="B9" s="5">
         <f>CODE(MID($B$5,B7,1))</f>
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ref="C9:K9" si="1">CODE(MID($B$5,C7,1))</f>
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
@@ -775,46 +778,46 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="8" t="str">
         <f>DEC2HEX(B9)</f>
-        <v>45</v>
-      </c>
-      <c r="C10" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8" t="str">
         <f>DEC2HEX(C9)</f>
-        <v>72</v>
-      </c>
-      <c r="D10" s="10" t="str">
+        <v>52</v>
+      </c>
+      <c r="D10" s="8" t="str">
         <f>DEC2HEX(D9)</f>
-        <v>72</v>
-      </c>
-      <c r="E10" s="10" t="str">
+        <v>48</v>
+      </c>
+      <c r="E10" s="8" t="str">
         <f>DEC2HEX(E9)</f>
-        <v>6F</v>
-      </c>
-      <c r="F10" s="10" t="str">
+        <v>3D</v>
+      </c>
+      <c r="F10" s="8" t="str">
         <f>DEC2HEX(F9)</f>
-        <v>72</v>
-      </c>
-      <c r="G10" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8" t="str">
         <f t="shared" ref="G10:K10" si="2">DEC2HEX(G9)</f>
-        <v>3D</v>
-      </c>
-      <c r="H10" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="H10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="I10" s="10" t="str">
+      <c r="I10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="J10" s="10" t="str">
+      <c r="J10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K10" s="10" t="str">
+      <c r="K10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -823,75 +826,75 @@
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="11">
         <f>256*C9+B9</f>
-        <v>29253</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8">
+        <v>21024</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11">
         <f t="shared" ref="D11:J11" si="3">256*E9+D9</f>
-        <v>28530</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
-        <f t="shared" si="3"/>
-        <v>15730</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
+        <v>15688</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11">
         <f t="shared" si="3"/>
         <v>8224</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11">
         <f t="shared" si="3"/>
         <v>8224</v>
       </c>
-      <c r="K11" s="8"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
+        <f t="shared" si="3"/>
+        <v>8224</v>
+      </c>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9" t="str">
+      <c r="A12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="12" t="str">
         <f>DEC2HEX(B11)</f>
-        <v>7245</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="str">
+        <v>5220</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="str">
         <f>DEC2HEX(D11)</f>
-        <v>6F72</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="str">
+        <v>3D48</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="str">
         <f>DEC2HEX(F11)</f>
-        <v>3D72</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9" t="str">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="str">
         <f>DEC2HEX(H11)</f>
         <v>2020</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9" t="str">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="str">
         <f>DEC2HEX(J11)</f>
         <v>2020</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="12"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="10">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>